<commit_message>
Fix in initial word
</commit_message>
<xml_diff>
--- a/statistics_by_word excel.xlsx
+++ b/statistics_by_word excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\federico.murphy\Documents\wordle-decipher\wordle_decipher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F729D734-43CB-417F-ABEC-75F8ABE6EE89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F5DDEC-3D1E-465A-B1A0-9E0437066394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total Percentage" sheetId="6" r:id="rId1"/>
@@ -4235,9 +4235,6 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4745,9 +4742,6 @@
       <c:pivotFmt>
         <c:idx val="9"/>
         <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -9146,8 +9140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9202A5F-78E7-4905-BFB6-D7DF986584EF}">
   <dimension ref="A3:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9615,8 +9609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52995EF-37C8-421F-8B77-A44BC1AF3B9E}">
   <dimension ref="A3:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>